<commit_message>
added title on board
</commit_message>
<xml_diff>
--- a/AIL/AIL_REV2/Released/BOM/Bill of Materials-AIL_REV2.xlsx
+++ b/AIL/AIL_REV2/Released/BOM/Bill of Materials-AIL_REV2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9466AE8D-1AF4-4547-8E44-1E159B42D124}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{22666E2F-2CE1-4089-ADE9-9D93FC24D335}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1956" windowWidth="17280" windowHeight="9024" xr2:uid="{D5AC2CAB-2135-4FC3-B658-9A94BAAFAF4A}"/>
+    <workbookView xWindow="0" yWindow="1956" windowWidth="17280" windowHeight="9024" xr2:uid="{251D694F-B0B9-4EAD-8A5C-7B7DB1406BF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-AIL_REV2" sheetId="1" r:id="rId1"/>
@@ -611,7 +611,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E692093-FFCA-4379-9D3A-2BF0E0692EF6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17AACEEF-BD61-4BFD-8005-24FD8E840160}">
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
added more gerber layers
</commit_message>
<xml_diff>
--- a/AIL/AIL_REV2/Released/BOM/Bill of Materials-AIL_REV2.xlsx
+++ b/AIL/AIL_REV2/Released/BOM/Bill of Materials-AIL_REV2.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{22666E2F-2CE1-4089-ADE9-9D93FC24D335}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FCB6FE73-C61A-4A87-83A2-58FC83E2037C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1956" windowWidth="17280" windowHeight="9024" xr2:uid="{251D694F-B0B9-4EAD-8A5C-7B7DB1406BF6}"/>
+    <workbookView xWindow="0" yWindow="1956" windowWidth="17280" windowHeight="9024" xr2:uid="{8D0EFE2D-E286-4568-81AF-7DE7D0E12F58}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-AIL_REV2" sheetId="1" r:id="rId1"/>
@@ -611,7 +611,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17AACEEF-BD61-4BFD-8005-24FD8E840160}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F7ACC8-ACC5-43C8-8819-CC277F662045}">
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>